<commit_message>
convert excel to pdf and save database
</commit_message>
<xml_diff>
--- a/Internfinder-BE/GAO_BackEnd/src/main/resources/jxls/template-hoanganh_demo.xlsx
+++ b/Internfinder-BE/GAO_BackEnd/src/main/resources/jxls/template-hoanganh_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAn_TN\GAO_BackEnd\Internfinder-BE\GAO_BackEnd\src\main\resources\jxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\D\GAO_BackEnd\Internfinder-BE\GAO_BackEnd\src\main\resources\jxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office ユーザー</author>
-    <author>NhanTQ</author>
+    <author>Hoàng Anh</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
@@ -44,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R14" authorId="1" shapeId="0">
+    <comment ref="E2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(var="education", items="user.educations", lastCell="R15")</t>
+          <t>jx:image(lastCell = "M9" src="user.image" imageType="JPEG")</t>
         </r>
       </text>
     </comment>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>${user.dayOfBirth}</t>
   </si>
@@ -88,19 +88,13 @@
     <t>OVERVIEW</t>
   </si>
   <si>
-    <t>${user.overView}</t>
-  </si>
-  <si>
     <t>View git</t>
   </si>
   <si>
-    <t>${user.firstName}   ${user.lastName}</t>
+    <t>${user.firstName} ${user.lastName}</t>
   </si>
   <si>
-    <t>${education.schoolName}</t>
-  </si>
-  <si>
-    <t>${education.startYear} to ${education.endYear}</t>
+    <t>Trần Hoàng Anh</t>
   </si>
 </sst>
 </file>
@@ -110,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,###&quot;円&quot;"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +175,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -267,7 +267,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -326,6 +326,24 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -335,9 +353,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,18 +361,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -425,58 +428,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95448</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47823</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="390525" y="323850"/>
-          <a:ext cx="1419423" cy="1419423"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100" cap="sq">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>26986</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -496,7 +447,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -540,7 +491,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -584,7 +535,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -875,10 +826,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CV31"/>
+  <dimension ref="A1:CV37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15:AY15"/>
+      <selection activeCell="BL10" sqref="BL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.85546875" defaultRowHeight="13.5" customHeight="1"/>
@@ -965,55 +916,46 @@
     <row r="3" spans="1:100" ht="19.5">
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="27" t="s">
-        <v>10</v>
+      <c r="P3" s="21" t="s">
+        <v>9</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="27"/>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="27"/>
-      <c r="AI3" s="27"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AM3" s="27"/>
-      <c r="AN3" s="27"/>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
-      <c r="AQ3" s="27"/>
-      <c r="AR3" s="27"/>
-      <c r="AS3" s="27"/>
-      <c r="AT3" s="27"/>
-      <c r="AU3" s="27"/>
-      <c r="AV3" s="27"/>
-      <c r="AW3" s="27"/>
-      <c r="AX3" s="27"/>
-      <c r="AY3" s="27"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="21"/>
+      <c r="AL3" s="21"/>
+      <c r="AM3" s="21"/>
+      <c r="AN3" s="21"/>
+      <c r="AO3" s="21"/>
+      <c r="AP3" s="21"/>
+      <c r="AQ3" s="21"/>
+      <c r="AR3" s="21"/>
+      <c r="AS3" s="21"/>
+      <c r="AT3" s="21"/>
+      <c r="AU3" s="21"/>
+      <c r="AV3" s="21"/>
+      <c r="AW3" s="21"/>
+      <c r="AX3" s="21"/>
+      <c r="AY3" s="21"/>
       <c r="AZ3" s="5"/>
       <c r="BA3" s="5"/>
     </row>
@@ -1021,53 +963,44 @@
       <c r="A4" s="2"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
-      <c r="AW4" s="27"/>
-      <c r="AX4" s="27"/>
-      <c r="AY4" s="27"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="21"/>
+      <c r="AR4" s="21"/>
+      <c r="AS4" s="21"/>
+      <c r="AT4" s="21"/>
+      <c r="AU4" s="21"/>
+      <c r="AV4" s="21"/>
+      <c r="AW4" s="21"/>
+      <c r="AX4" s="21"/>
+      <c r="AY4" s="21"/>
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
       <c r="CV4" s="3"/>
@@ -1075,53 +1008,44 @@
     <row r="5" spans="1:100" ht="15">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="27"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="27"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="27"/>
-      <c r="AM5" s="27"/>
-      <c r="AN5" s="27"/>
-      <c r="AO5" s="27"/>
-      <c r="AP5" s="27"/>
-      <c r="AQ5" s="27"/>
-      <c r="AR5" s="27"/>
-      <c r="AS5" s="27"/>
-      <c r="AT5" s="27"/>
-      <c r="AU5" s="27"/>
-      <c r="AV5" s="27"/>
-      <c r="AW5" s="27"/>
-      <c r="AX5" s="27"/>
-      <c r="AY5" s="27"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="21"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="21"/>
+      <c r="AO5" s="21"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="21"/>
+      <c r="AR5" s="21"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="21"/>
+      <c r="AU5" s="21"/>
+      <c r="AV5" s="21"/>
+      <c r="AW5" s="21"/>
+      <c r="AX5" s="21"/>
+      <c r="AY5" s="21"/>
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
     </row>
@@ -1130,68 +1054,68 @@
       <c r="CV6" s="3"/>
     </row>
     <row r="7" spans="1:100" ht="15">
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="23"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="22"/>
       <c r="AM7" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:100" ht="15">
       <c r="A8" s="2"/>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="22"/>
     </row>
     <row r="9" spans="1:100" ht="15">
-      <c r="R9" s="23" t="s">
+      <c r="R9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
     </row>
     <row r="10" spans="1:100" ht="15">
       <c r="A10" s="2"/>
@@ -1265,58 +1189,58 @@
     </row>
     <row r="12" spans="1:100" ht="18">
       <c r="A12" s="2"/>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="29"/>
-      <c r="R12" s="30" t="s">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="24"/>
+      <c r="R12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="30"/>
-      <c r="AA12" s="30"/>
-      <c r="AB12" s="30"/>
-      <c r="AC12" s="30"/>
-      <c r="AD12" s="30"/>
-      <c r="AE12" s="30"/>
-      <c r="AF12" s="30"/>
-      <c r="AG12" s="30"/>
-      <c r="AH12" s="30"/>
-      <c r="AI12" s="30"/>
-      <c r="AJ12" s="30"/>
-      <c r="AK12" s="30"/>
-      <c r="AL12" s="30"/>
-      <c r="AM12" s="30"/>
-      <c r="AN12" s="30"/>
-      <c r="AO12" s="30"/>
-      <c r="AP12" s="30"/>
-      <c r="AQ12" s="30"/>
-      <c r="AR12" s="30"/>
-      <c r="AS12" s="30"/>
-      <c r="AT12" s="30"/>
-      <c r="AU12" s="30"/>
-      <c r="AV12" s="30"/>
-      <c r="AW12" s="30"/>
-      <c r="AX12" s="30"/>
-      <c r="AY12" s="30"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="25"/>
+      <c r="AD12" s="25"/>
+      <c r="AE12" s="25"/>
+      <c r="AF12" s="25"/>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="25"/>
+      <c r="AJ12" s="25"/>
+      <c r="AK12" s="25"/>
+      <c r="AL12" s="25"/>
+      <c r="AM12" s="25"/>
+      <c r="AN12" s="25"/>
+      <c r="AO12" s="25"/>
+      <c r="AP12" s="25"/>
+      <c r="AQ12" s="25"/>
+      <c r="AR12" s="25"/>
+      <c r="AS12" s="25"/>
+      <c r="AT12" s="25"/>
+      <c r="AU12" s="25"/>
+      <c r="AV12" s="25"/>
+      <c r="AW12" s="25"/>
+      <c r="AX12" s="25"/>
+      <c r="AY12" s="25"/>
     </row>
     <row r="13" spans="1:100" ht="15">
       <c r="C13" s="10"/>
@@ -1336,127 +1260,123 @@
     </row>
     <row r="14" spans="1:100" ht="15">
       <c r="A14" s="2"/>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-      <c r="R14" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="22"/>
-      <c r="AB14" s="22"/>
-      <c r="AC14" s="22"/>
-      <c r="AD14" s="22"/>
-      <c r="AE14" s="22"/>
-      <c r="AF14" s="22"/>
-      <c r="AG14" s="22"/>
-      <c r="AH14" s="22"/>
-      <c r="AI14" s="22"/>
-      <c r="AJ14" s="22"/>
-      <c r="AK14" s="22"/>
-      <c r="AL14" s="22"/>
-      <c r="AM14" s="22"/>
-      <c r="AN14" s="22"/>
-      <c r="AO14" s="22"/>
-      <c r="AP14" s="22"/>
-      <c r="AQ14" s="22"/>
-      <c r="AR14" s="22"/>
-      <c r="AS14" s="22"/>
-      <c r="AT14" s="22"/>
-      <c r="AU14" s="22"/>
-      <c r="AV14" s="22"/>
-      <c r="AW14" s="22"/>
-      <c r="AX14" s="22"/>
-      <c r="AY14" s="22"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="27"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="28"/>
+      <c r="AH14" s="28"/>
+      <c r="AI14" s="28"/>
+      <c r="AJ14" s="28"/>
+      <c r="AK14" s="28"/>
+      <c r="AL14" s="28"/>
+      <c r="AM14" s="28"/>
+      <c r="AN14" s="28"/>
+      <c r="AO14" s="28"/>
+      <c r="AP14" s="28"/>
+      <c r="AQ14" s="28"/>
+      <c r="AR14" s="28"/>
+      <c r="AS14" s="28"/>
+      <c r="AT14" s="28"/>
+      <c r="AU14" s="28"/>
+      <c r="AV14" s="28"/>
+      <c r="AW14" s="28"/>
+      <c r="AX14" s="28"/>
+      <c r="AY14" s="28"/>
     </row>
     <row r="15" spans="1:100" ht="15">
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="R15" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-      <c r="AE15" s="23"/>
-      <c r="AF15" s="23"/>
-      <c r="AG15" s="23"/>
-      <c r="AH15" s="23"/>
-      <c r="AI15" s="23"/>
-      <c r="AJ15" s="23"/>
-      <c r="AK15" s="23"/>
-      <c r="AL15" s="23"/>
-      <c r="AM15" s="23"/>
-      <c r="AN15" s="23"/>
-      <c r="AO15" s="23"/>
-      <c r="AP15" s="23"/>
-      <c r="AQ15" s="23"/>
-      <c r="AR15" s="23"/>
-      <c r="AS15" s="23"/>
-      <c r="AT15" s="23"/>
-      <c r="AU15" s="23"/>
-      <c r="AV15" s="23"/>
-      <c r="AW15" s="23"/>
-      <c r="AX15" s="23"/>
-      <c r="AY15" s="23"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="27"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
+      <c r="AA15" s="22"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+      <c r="AD15" s="22"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
+      <c r="AH15" s="22"/>
+      <c r="AI15" s="22"/>
+      <c r="AJ15" s="22"/>
+      <c r="AK15" s="22"/>
+      <c r="AL15" s="22"/>
+      <c r="AM15" s="22"/>
+      <c r="AN15" s="22"/>
+      <c r="AO15" s="22"/>
+      <c r="AP15" s="22"/>
+      <c r="AQ15" s="22"/>
+      <c r="AR15" s="22"/>
+      <c r="AS15" s="22"/>
+      <c r="AT15" s="22"/>
+      <c r="AU15" s="22"/>
+      <c r="AV15" s="22"/>
+      <c r="AW15" s="22"/>
+      <c r="AX15" s="22"/>
+      <c r="AY15" s="22"/>
     </row>
     <row r="16" spans="1:100" ht="15">
       <c r="A16" s="2"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="27"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
@@ -1498,20 +1418,20 @@
       <c r="BC16" s="12"/>
     </row>
     <row r="17" spans="1:55" ht="15">
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="27"/>
       <c r="Q17" s="12"/>
       <c r="R17" s="13"/>
       <c r="S17" s="13"/>
@@ -1554,20 +1474,20 @@
     </row>
     <row r="18" spans="1:55" ht="15">
       <c r="A18" s="2"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="27"/>
       <c r="Q18" s="12"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -1609,20 +1529,20 @@
       <c r="BC18" s="12"/>
     </row>
     <row r="19" spans="1:55" ht="15">
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="27"/>
       <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -1664,20 +1584,20 @@
       <c r="BC19" s="12"/>
     </row>
     <row r="20" spans="1:55" ht="15">
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="14"/>
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
@@ -1719,72 +1639,72 @@
       <c r="BC20" s="12"/>
     </row>
     <row r="21" spans="1:55" ht="15">
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="21"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="27"/>
     </row>
     <row r="22" spans="1:55" ht="15">
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="21"/>
-      <c r="R22" s="24" t="s">
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="27"/>
+      <c r="R22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="24"/>
-      <c r="AD22" s="24"/>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="24"/>
-      <c r="AG22" s="24"/>
-      <c r="AH22" s="24"/>
-      <c r="AI22" s="24"/>
-      <c r="AJ22" s="24"/>
-      <c r="AK22" s="24"/>
-      <c r="AL22" s="24"/>
-      <c r="AM22" s="24"/>
-      <c r="AN22" s="24"/>
-      <c r="AO22" s="24"/>
-      <c r="AP22" s="24"/>
-      <c r="AQ22" s="24"/>
-      <c r="AR22" s="24"/>
-      <c r="AS22" s="24"/>
-      <c r="AT22" s="24"/>
-      <c r="AU22" s="24"/>
-      <c r="AV22" s="24"/>
-      <c r="AW22" s="24"/>
-      <c r="AX22" s="24"/>
-      <c r="AY22" s="24"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="29"/>
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="29"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="29"/>
+      <c r="AM22" s="29"/>
+      <c r="AN22" s="29"/>
+      <c r="AO22" s="29"/>
+      <c r="AP22" s="29"/>
+      <c r="AQ22" s="29"/>
+      <c r="AR22" s="29"/>
+      <c r="AS22" s="29"/>
+      <c r="AT22" s="29"/>
+      <c r="AU22" s="29"/>
+      <c r="AV22" s="29"/>
+      <c r="AW22" s="29"/>
+      <c r="AX22" s="29"/>
+      <c r="AY22" s="29"/>
     </row>
     <row r="23" spans="1:55" ht="15">
       <c r="C23" s="10"/>
@@ -1817,94 +1737,92 @@
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
-      <c r="R24" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="25"/>
-      <c r="X24" s="25"/>
-      <c r="Y24" s="25"/>
-      <c r="Z24" s="25"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="25"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="25"/>
-      <c r="AE24" s="25"/>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="25"/>
-      <c r="AH24" s="25"/>
-      <c r="AI24" s="25"/>
-      <c r="AJ24" s="25"/>
-      <c r="AK24" s="25"/>
-      <c r="AL24" s="25"/>
-      <c r="AM24" s="25"/>
-      <c r="AN24" s="25"/>
-      <c r="AO24" s="25"/>
-      <c r="AP24" s="25"/>
-      <c r="AQ24" s="25"/>
-      <c r="AR24" s="25"/>
-      <c r="AS24" s="25"/>
-      <c r="AT24" s="25"/>
-      <c r="AU24" s="25"/>
-      <c r="AV24" s="25"/>
-      <c r="AW24" s="25"/>
-      <c r="AX24" s="25"/>
-      <c r="AY24" s="25"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
+      <c r="AA24" s="30"/>
+      <c r="AB24" s="30"/>
+      <c r="AC24" s="30"/>
+      <c r="AD24" s="30"/>
+      <c r="AE24" s="30"/>
+      <c r="AF24" s="30"/>
+      <c r="AG24" s="30"/>
+      <c r="AH24" s="30"/>
+      <c r="AI24" s="30"/>
+      <c r="AJ24" s="30"/>
+      <c r="AK24" s="30"/>
+      <c r="AL24" s="30"/>
+      <c r="AM24" s="30"/>
+      <c r="AN24" s="30"/>
+      <c r="AO24" s="30"/>
+      <c r="AP24" s="30"/>
+      <c r="AQ24" s="30"/>
+      <c r="AR24" s="30"/>
+      <c r="AS24" s="30"/>
+      <c r="AT24" s="30"/>
+      <c r="AU24" s="30"/>
+      <c r="AV24" s="30"/>
+      <c r="AW24" s="30"/>
+      <c r="AX24" s="30"/>
+      <c r="AY24" s="30"/>
     </row>
     <row r="25" spans="1:55" ht="15">
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="26" t="s">
-        <v>9</v>
+      <c r="F25" s="31" t="s">
+        <v>8</v>
       </c>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="25"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="25"/>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
-      <c r="AB25" s="25"/>
-      <c r="AC25" s="25"/>
-      <c r="AD25" s="25"/>
-      <c r="AE25" s="25"/>
-      <c r="AF25" s="25"/>
-      <c r="AG25" s="25"/>
-      <c r="AH25" s="25"/>
-      <c r="AI25" s="25"/>
-      <c r="AJ25" s="25"/>
-      <c r="AK25" s="25"/>
-      <c r="AL25" s="25"/>
-      <c r="AM25" s="25"/>
-      <c r="AN25" s="25"/>
-      <c r="AO25" s="25"/>
-      <c r="AP25" s="25"/>
-      <c r="AQ25" s="25"/>
-      <c r="AR25" s="25"/>
-      <c r="AS25" s="25"/>
-      <c r="AT25" s="25"/>
-      <c r="AU25" s="25"/>
-      <c r="AV25" s="25"/>
-      <c r="AW25" s="25"/>
-      <c r="AX25" s="25"/>
-      <c r="AY25" s="25"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="30"/>
+      <c r="AA25" s="30"/>
+      <c r="AB25" s="30"/>
+      <c r="AC25" s="30"/>
+      <c r="AD25" s="30"/>
+      <c r="AE25" s="30"/>
+      <c r="AF25" s="30"/>
+      <c r="AG25" s="30"/>
+      <c r="AH25" s="30"/>
+      <c r="AI25" s="30"/>
+      <c r="AJ25" s="30"/>
+      <c r="AK25" s="30"/>
+      <c r="AL25" s="30"/>
+      <c r="AM25" s="30"/>
+      <c r="AN25" s="30"/>
+      <c r="AO25" s="30"/>
+      <c r="AP25" s="30"/>
+      <c r="AQ25" s="30"/>
+      <c r="AR25" s="30"/>
+      <c r="AS25" s="30"/>
+      <c r="AT25" s="30"/>
+      <c r="AU25" s="30"/>
+      <c r="AV25" s="30"/>
+      <c r="AW25" s="30"/>
+      <c r="AX25" s="30"/>
+      <c r="AY25" s="30"/>
     </row>
     <row r="26" spans="1:55" ht="15">
       <c r="A26" s="16"/>
@@ -1912,52 +1830,52 @@
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="17"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="25"/>
-      <c r="V26" s="25"/>
-      <c r="W26" s="25"/>
-      <c r="X26" s="25"/>
-      <c r="Y26" s="25"/>
-      <c r="Z26" s="25"/>
-      <c r="AA26" s="25"/>
-      <c r="AB26" s="25"/>
-      <c r="AC26" s="25"/>
-      <c r="AD26" s="25"/>
-      <c r="AE26" s="25"/>
-      <c r="AF26" s="25"/>
-      <c r="AG26" s="25"/>
-      <c r="AH26" s="25"/>
-      <c r="AI26" s="25"/>
-      <c r="AJ26" s="25"/>
-      <c r="AK26" s="25"/>
-      <c r="AL26" s="25"/>
-      <c r="AM26" s="25"/>
-      <c r="AN26" s="25"/>
-      <c r="AO26" s="25"/>
-      <c r="AP26" s="25"/>
-      <c r="AQ26" s="25"/>
-      <c r="AR26" s="25"/>
-      <c r="AS26" s="25"/>
-      <c r="AT26" s="25"/>
-      <c r="AU26" s="25"/>
-      <c r="AV26" s="25"/>
-      <c r="AW26" s="25"/>
-      <c r="AX26" s="25"/>
-      <c r="AY26" s="25"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="30"/>
+      <c r="AA26" s="30"/>
+      <c r="AB26" s="30"/>
+      <c r="AC26" s="30"/>
+      <c r="AD26" s="30"/>
+      <c r="AE26" s="30"/>
+      <c r="AF26" s="30"/>
+      <c r="AG26" s="30"/>
+      <c r="AH26" s="30"/>
+      <c r="AI26" s="30"/>
+      <c r="AJ26" s="30"/>
+      <c r="AK26" s="30"/>
+      <c r="AL26" s="30"/>
+      <c r="AM26" s="30"/>
+      <c r="AN26" s="30"/>
+      <c r="AO26" s="30"/>
+      <c r="AP26" s="30"/>
+      <c r="AQ26" s="30"/>
+      <c r="AR26" s="30"/>
+      <c r="AS26" s="30"/>
+      <c r="AT26" s="30"/>
+      <c r="AU26" s="30"/>
+      <c r="AV26" s="30"/>
+      <c r="AW26" s="30"/>
+      <c r="AX26" s="30"/>
+      <c r="AY26" s="30"/>
       <c r="AZ26" s="19"/>
       <c r="BA26" s="19"/>
       <c r="BB26" s="19"/>
@@ -1978,40 +1896,40 @@
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
-      <c r="AD27" s="25"/>
-      <c r="AE27" s="25"/>
-      <c r="AF27" s="25"/>
-      <c r="AG27" s="25"/>
-      <c r="AH27" s="25"/>
-      <c r="AI27" s="25"/>
-      <c r="AJ27" s="25"/>
-      <c r="AK27" s="25"/>
-      <c r="AL27" s="25"/>
-      <c r="AM27" s="25"/>
-      <c r="AN27" s="25"/>
-      <c r="AO27" s="25"/>
-      <c r="AP27" s="25"/>
-      <c r="AQ27" s="25"/>
-      <c r="AR27" s="25"/>
-      <c r="AS27" s="25"/>
-      <c r="AT27" s="25"/>
-      <c r="AU27" s="25"/>
-      <c r="AV27" s="25"/>
-      <c r="AW27" s="25"/>
-      <c r="AX27" s="25"/>
-      <c r="AY27" s="25"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
+      <c r="AA27" s="30"/>
+      <c r="AB27" s="30"/>
+      <c r="AC27" s="30"/>
+      <c r="AD27" s="30"/>
+      <c r="AE27" s="30"/>
+      <c r="AF27" s="30"/>
+      <c r="AG27" s="30"/>
+      <c r="AH27" s="30"/>
+      <c r="AI27" s="30"/>
+      <c r="AJ27" s="30"/>
+      <c r="AK27" s="30"/>
+      <c r="AL27" s="30"/>
+      <c r="AM27" s="30"/>
+      <c r="AN27" s="30"/>
+      <c r="AO27" s="30"/>
+      <c r="AP27" s="30"/>
+      <c r="AQ27" s="30"/>
+      <c r="AR27" s="30"/>
+      <c r="AS27" s="30"/>
+      <c r="AT27" s="30"/>
+      <c r="AU27" s="30"/>
+      <c r="AV27" s="30"/>
+      <c r="AW27" s="30"/>
+      <c r="AX27" s="30"/>
+      <c r="AY27" s="30"/>
     </row>
     <row r="28" spans="1:55" ht="15">
       <c r="C28" s="10"/>
@@ -2028,40 +1946,40 @@
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="25"/>
-      <c r="AB28" s="25"/>
-      <c r="AC28" s="25"/>
-      <c r="AD28" s="25"/>
-      <c r="AE28" s="25"/>
-      <c r="AF28" s="25"/>
-      <c r="AG28" s="25"/>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="25"/>
-      <c r="AJ28" s="25"/>
-      <c r="AK28" s="25"/>
-      <c r="AL28" s="25"/>
-      <c r="AM28" s="25"/>
-      <c r="AN28" s="25"/>
-      <c r="AO28" s="25"/>
-      <c r="AP28" s="25"/>
-      <c r="AQ28" s="25"/>
-      <c r="AR28" s="25"/>
-      <c r="AS28" s="25"/>
-      <c r="AT28" s="25"/>
-      <c r="AU28" s="25"/>
-      <c r="AV28" s="25"/>
-      <c r="AW28" s="25"/>
-      <c r="AX28" s="25"/>
-      <c r="AY28" s="25"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+      <c r="AA28" s="30"/>
+      <c r="AB28" s="30"/>
+      <c r="AC28" s="30"/>
+      <c r="AD28" s="30"/>
+      <c r="AE28" s="30"/>
+      <c r="AF28" s="30"/>
+      <c r="AG28" s="30"/>
+      <c r="AH28" s="30"/>
+      <c r="AI28" s="30"/>
+      <c r="AJ28" s="30"/>
+      <c r="AK28" s="30"/>
+      <c r="AL28" s="30"/>
+      <c r="AM28" s="30"/>
+      <c r="AN28" s="30"/>
+      <c r="AO28" s="30"/>
+      <c r="AP28" s="30"/>
+      <c r="AQ28" s="30"/>
+      <c r="AR28" s="30"/>
+      <c r="AS28" s="30"/>
+      <c r="AT28" s="30"/>
+      <c r="AU28" s="30"/>
+      <c r="AV28" s="30"/>
+      <c r="AW28" s="30"/>
+      <c r="AX28" s="30"/>
+      <c r="AY28" s="30"/>
     </row>
     <row r="29" spans="1:55" ht="15">
       <c r="C29" s="10"/>
@@ -2078,40 +1996,40 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
-      <c r="AA29" s="25"/>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="25"/>
-      <c r="AD29" s="25"/>
-      <c r="AE29" s="25"/>
-      <c r="AF29" s="25"/>
-      <c r="AG29" s="25"/>
-      <c r="AH29" s="25"/>
-      <c r="AI29" s="25"/>
-      <c r="AJ29" s="25"/>
-      <c r="AK29" s="25"/>
-      <c r="AL29" s="25"/>
-      <c r="AM29" s="25"/>
-      <c r="AN29" s="25"/>
-      <c r="AO29" s="25"/>
-      <c r="AP29" s="25"/>
-      <c r="AQ29" s="25"/>
-      <c r="AR29" s="25"/>
-      <c r="AS29" s="25"/>
-      <c r="AT29" s="25"/>
-      <c r="AU29" s="25"/>
-      <c r="AV29" s="25"/>
-      <c r="AW29" s="25"/>
-      <c r="AX29" s="25"/>
-      <c r="AY29" s="25"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="30"/>
+      <c r="Z29" s="30"/>
+      <c r="AA29" s="30"/>
+      <c r="AB29" s="30"/>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="30"/>
+      <c r="AE29" s="30"/>
+      <c r="AF29" s="30"/>
+      <c r="AG29" s="30"/>
+      <c r="AH29" s="30"/>
+      <c r="AI29" s="30"/>
+      <c r="AJ29" s="30"/>
+      <c r="AK29" s="30"/>
+      <c r="AL29" s="30"/>
+      <c r="AM29" s="30"/>
+      <c r="AN29" s="30"/>
+      <c r="AO29" s="30"/>
+      <c r="AP29" s="30"/>
+      <c r="AQ29" s="30"/>
+      <c r="AR29" s="30"/>
+      <c r="AS29" s="30"/>
+      <c r="AT29" s="30"/>
+      <c r="AU29" s="30"/>
+      <c r="AV29" s="30"/>
+      <c r="AW29" s="30"/>
+      <c r="AX29" s="30"/>
+      <c r="AY29" s="30"/>
     </row>
     <row r="30" spans="1:55" ht="15">
       <c r="C30" s="10"/>
@@ -2128,40 +2046,40 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="11"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
-      <c r="V30" s="25"/>
-      <c r="W30" s="25"/>
-      <c r="X30" s="25"/>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
-      <c r="AA30" s="25"/>
-      <c r="AB30" s="25"/>
-      <c r="AC30" s="25"/>
-      <c r="AD30" s="25"/>
-      <c r="AE30" s="25"/>
-      <c r="AF30" s="25"/>
-      <c r="AG30" s="25"/>
-      <c r="AH30" s="25"/>
-      <c r="AI30" s="25"/>
-      <c r="AJ30" s="25"/>
-      <c r="AK30" s="25"/>
-      <c r="AL30" s="25"/>
-      <c r="AM30" s="25"/>
-      <c r="AN30" s="25"/>
-      <c r="AO30" s="25"/>
-      <c r="AP30" s="25"/>
-      <c r="AQ30" s="25"/>
-      <c r="AR30" s="25"/>
-      <c r="AS30" s="25"/>
-      <c r="AT30" s="25"/>
-      <c r="AU30" s="25"/>
-      <c r="AV30" s="25"/>
-      <c r="AW30" s="25"/>
-      <c r="AX30" s="25"/>
-      <c r="AY30" s="25"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="30"/>
+      <c r="Z30" s="30"/>
+      <c r="AA30" s="30"/>
+      <c r="AB30" s="30"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="30"/>
+      <c r="AF30" s="30"/>
+      <c r="AG30" s="30"/>
+      <c r="AH30" s="30"/>
+      <c r="AI30" s="30"/>
+      <c r="AJ30" s="30"/>
+      <c r="AK30" s="30"/>
+      <c r="AL30" s="30"/>
+      <c r="AM30" s="30"/>
+      <c r="AN30" s="30"/>
+      <c r="AO30" s="30"/>
+      <c r="AP30" s="30"/>
+      <c r="AQ30" s="30"/>
+      <c r="AR30" s="30"/>
+      <c r="AS30" s="30"/>
+      <c r="AT30" s="30"/>
+      <c r="AU30" s="30"/>
+      <c r="AV30" s="30"/>
+      <c r="AW30" s="30"/>
+      <c r="AX30" s="30"/>
+      <c r="AY30" s="30"/>
     </row>
     <row r="31" spans="1:55" ht="15">
       <c r="C31" s="10"/>
@@ -2178,55 +2096,60 @@
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
       <c r="P31" s="11"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
-      <c r="V31" s="25"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="25"/>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AA31" s="25"/>
-      <c r="AB31" s="25"/>
-      <c r="AC31" s="25"/>
-      <c r="AD31" s="25"/>
-      <c r="AE31" s="25"/>
-      <c r="AF31" s="25"/>
-      <c r="AG31" s="25"/>
-      <c r="AH31" s="25"/>
-      <c r="AI31" s="25"/>
-      <c r="AJ31" s="25"/>
-      <c r="AK31" s="25"/>
-      <c r="AL31" s="25"/>
-      <c r="AM31" s="25"/>
-      <c r="AN31" s="25"/>
-      <c r="AO31" s="25"/>
-      <c r="AP31" s="25"/>
-      <c r="AQ31" s="25"/>
-      <c r="AR31" s="25"/>
-      <c r="AS31" s="25"/>
-      <c r="AT31" s="25"/>
-      <c r="AU31" s="25"/>
-      <c r="AV31" s="25"/>
-      <c r="AW31" s="25"/>
-      <c r="AX31" s="25"/>
-      <c r="AY31" s="25"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+      <c r="X31" s="30"/>
+      <c r="Y31" s="30"/>
+      <c r="Z31" s="30"/>
+      <c r="AA31" s="30"/>
+      <c r="AB31" s="30"/>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="30"/>
+      <c r="AE31" s="30"/>
+      <c r="AF31" s="30"/>
+      <c r="AG31" s="30"/>
+      <c r="AH31" s="30"/>
+      <c r="AI31" s="30"/>
+      <c r="AJ31" s="30"/>
+      <c r="AK31" s="30"/>
+      <c r="AL31" s="30"/>
+      <c r="AM31" s="30"/>
+      <c r="AN31" s="30"/>
+      <c r="AO31" s="30"/>
+      <c r="AP31" s="30"/>
+      <c r="AQ31" s="30"/>
+      <c r="AR31" s="30"/>
+      <c r="AS31" s="30"/>
+      <c r="AT31" s="30"/>
+      <c r="AU31" s="30"/>
+      <c r="AV31" s="30"/>
+      <c r="AW31" s="30"/>
+      <c r="AX31" s="30"/>
+      <c r="AY31" s="30"/>
+    </row>
+    <row r="37" spans="52:52" ht="13.5" customHeight="1">
+      <c r="AZ37" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C14:P22"/>
+    <mergeCell ref="R14:AY14"/>
+    <mergeCell ref="R15:AY15"/>
+    <mergeCell ref="R22:AY22"/>
+    <mergeCell ref="R24:AY31"/>
+    <mergeCell ref="F25:M26"/>
     <mergeCell ref="P3:AY5"/>
     <mergeCell ref="R7:AG7"/>
     <mergeCell ref="R8:AG8"/>
     <mergeCell ref="R9:AG9"/>
     <mergeCell ref="C12:P12"/>
     <mergeCell ref="R12:AY12"/>
-    <mergeCell ref="C14:P22"/>
-    <mergeCell ref="R14:AY14"/>
-    <mergeCell ref="R15:AY15"/>
-    <mergeCell ref="R22:AY22"/>
-    <mergeCell ref="R24:AY31"/>
-    <mergeCell ref="F25:M26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F25:M26" r:id="rId1" display="View git"/>

</xml_diff>